<commit_message>
Add initial plan of mobile
</commit_message>
<xml_diff>
--- a/docs/Wave23_Plan_Corelia.xlsx
+++ b/docs/Wave23_Plan_Corelia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\_Work\corelia\_Intern\intern\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B449C3D4-277B-44C0-9D07-B889F640970E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4736B6F6-D6C7-47A5-8ACE-42F9F17F2159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wave 23 - Plan" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="155">
   <si>
     <t>Data Science</t>
   </si>
@@ -455,9 +455,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>Ameen</t>
-  </si>
-  <si>
     <t>Bootstrap, Fonts,,,</t>
   </si>
   <si>
@@ -467,9 +464,6 @@
     <t>Month of Feb BECS1</t>
   </si>
   <si>
-    <t>Ziad/Emad</t>
-  </si>
-  <si>
     <t>DMS persentation</t>
   </si>
   <si>
@@ -477,6 +471,27 @@
   </si>
   <si>
     <t>Month of Feb DS1-2</t>
+  </si>
+  <si>
+    <t>Ameen/Nabil</t>
+  </si>
+  <si>
+    <t>Development(Mobile)</t>
+  </si>
+  <si>
+    <t>Dart</t>
+  </si>
+  <si>
+    <t>Mob1</t>
+  </si>
+  <si>
+    <t>Ziad</t>
+  </si>
+  <si>
+    <t>Aya</t>
+  </si>
+  <si>
+    <t>Month of Feb Mob1</t>
   </si>
 </sst>
 </file>
@@ -626,15 +641,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -978,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83ECA02-392D-44CC-A350-86FD530A6FE6}">
-  <dimension ref="A1:AL33"/>
+  <dimension ref="A1:AL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1016,39 +1031,39 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
@@ -1524,13 +1539,13 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="9" t="s">
+      <c r="O22" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
     </row>
     <row r="23" spans="10:19" x14ac:dyDescent="0.25">
       <c r="J23" s="4" t="s">
@@ -1662,9 +1677,73 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="13:19" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+    </row>
+    <row r="39" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="M39" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="R39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="S39" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="N40" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="P40" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S40" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="R41" s="7"/>
+    </row>
+    <row r="45" spans="13:19" x14ac:dyDescent="0.25">
+      <c r="O45" s="7"/>
+    </row>
+    <row r="54" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P54" s="7"/>
+    </row>
+    <row r="55" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P55" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="O38:S38"/>
     <mergeCell ref="O22:S22"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="AA1:AB1"/>
@@ -1695,14 +1774,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="A1" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1954,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85253843-A484-4398-A3E8-7BE978F9AC63}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1965,684 +2044,924 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.375" customWidth="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="10"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="N1" s="9"/>
+      <c r="O1" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="9"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+      <c r="N2" s="9"/>
+      <c r="O2" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="9"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U10" s="9"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="9"/>
+      <c r="O16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="R16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="9"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10" t="s">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="O1:R1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add fastapi session materials
</commit_message>
<xml_diff>
--- a/docs/Wave23_Plan_Corelia.xlsx
+++ b/docs/Wave23_Plan_Corelia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\_Work\corelia\_Intern\intern\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0839757F-4DCB-4589-98B0-CED31B079F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1530C11D-2DC7-4A2F-8938-67193CB83599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wave 23 - Plan" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="202">
   <si>
     <t>Data Science</t>
   </si>
@@ -624,6 +624,15 @@
   </si>
   <si>
     <t>Identity - Roles</t>
+  </si>
+  <si>
+    <t>API of Models</t>
+  </si>
+  <si>
+    <t>DB : Finish Models, entitles, ..</t>
+  </si>
+  <si>
+    <t>Auth : FInish  Rules, Identity</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83ECA02-392D-44CC-A350-86FD530A6FE6}">
   <dimension ref="A1:AL55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="91" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
@@ -2192,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85253843-A484-4398-A3E8-7BE978F9AC63}">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -2754,20 +2763,29 @@
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:20" ht="19.05" x14ac:dyDescent="0.35">
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
+      <c r="M24" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="25" spans="7:20" x14ac:dyDescent="0.25">
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
+      <c r="N25" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="26" spans="7:20" x14ac:dyDescent="0.25">
       <c r="I26" s="9"/>
@@ -2788,7 +2806,44 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
+    </row>
+    <row r="29" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>200</v>
+      </c>
+      <c r="N29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>201</v>
+      </c>
+      <c r="N30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M34" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>199</v>
+      </c>
+      <c r="N35" t="s">
+        <v>192</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>